<commit_message>
SSDM-55: The last update of xls test data
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-vocabulary-property-compatible-with-import.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-vocabulary-property-compatible-with-import.xlsx
@@ -311,10 +311,10 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
SSDM-55: xls test data fixes
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-vocabulary-property-compatible-with-import.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-vocabulary-property-compatible-with-import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="44">
   <si>
     <t xml:space="preserve">VOCABULARY_TYPE</t>
   </si>
@@ -118,6 +118,9 @@
     <t xml:space="preserve">$NAME</t>
   </si>
   <si>
+    <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">General info</t>
   </si>
   <si>
@@ -125,9 +128,6 @@
   </si>
   <si>
     <t xml:space="preserve">VARCHAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">$BARCODE</t>
@@ -158,9 +158,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -250,7 +249,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -276,10 +275,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -311,10 +306,10 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -486,28 +481,26 @@
       <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>35</v>
+      <c r="L13" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,28 +510,26 @@
       <c r="B14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L14" s="8" t="s">
-        <v>35</v>
+      <c r="L14" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,16 +539,14 @@
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>38</v>
@@ -571,12 +560,12 @@
       <c r="I15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="8" t="s">
-        <v>35</v>
+      <c r="L15" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="9"/>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -618,9 +607,8 @@
       <c r="C19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="D19" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>43</v>
@@ -671,28 +659,26 @@
       <c r="B21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>35</v>
+      <c r="L21" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,28 +688,26 @@
       <c r="B22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L22" s="8" t="s">
-        <v>35</v>
+      <c r="L22" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -733,16 +717,14 @@
       <c r="B23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>38</v>
@@ -756,8 +738,8 @@
       <c r="I23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L23" s="8" t="s">
-        <v>35</v>
+      <c r="L23" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>